<commit_message>
Model for sale is create
</commit_message>
<xml_diff>
--- a/TotalSalebyBrand.xlsx
+++ b/TotalSalebyBrand.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xvw41\Desktop\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B1E734-F9D8-4BE3-A6BC-08848BE15D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB61A78-8453-4B4B-8AE8-C033EE210C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92CFF864-5EC4-49B0-8669-4780DAA45A52}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="34">
   <si>
     <t>Ford</t>
   </si>
@@ -69,14 +69,6 @@
   </si>
   <si>
     <t>Jaguar</t>
-  </si>
-  <si>
-    <t>CurrentYearSales</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LastYearSales</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Month</t>
@@ -140,7 +132,20 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Mercedes *3</t>
+    <t>2019Sales</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020Sales</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018Sales</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mercedes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -507,11 +512,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29C4026-0F90-48FB-97CF-A26CF56F906F}">
-  <dimension ref="A1:D265"/>
+  <dimension ref="A1:E265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="121" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -520,23 +523,26 @@
     <col min="3" max="3" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>295536</v>
@@ -544,13 +550,16 @@
       <c r="C2" s="1">
         <v>277640</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
+        <v>296632</v>
+      </c>
+      <c r="E2">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1">
         <v>251256</v>
@@ -558,11 +567,14 @@
       <c r="C3" s="1">
         <v>207373</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
+        <v>220910</v>
+      </c>
+      <c r="E3">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -572,13 +584,16 @@
       <c r="C4" s="1">
         <v>216439</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
+        <v>219632</v>
+      </c>
+      <c r="E4">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>202371</v>
@@ -586,11 +601,14 @@
       <c r="C5" s="1">
         <v>191075</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
+        <v>196520</v>
+      </c>
+      <c r="E5">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -600,13 +618,16 @@
       <c r="C6" s="1">
         <v>136566</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
+        <v>155115</v>
+      </c>
+      <c r="E6">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
         <v>98638</v>
@@ -614,11 +635,14 @@
       <c r="C7" s="1">
         <v>104781</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
+        <v>148720</v>
+      </c>
+      <c r="E7">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -628,11 +652,14 @@
       <c r="C8" s="1">
         <v>66945</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
+        <v>65721</v>
+      </c>
+      <c r="E8">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -642,11 +669,14 @@
       <c r="C9" s="1">
         <v>62364</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
+        <v>64541</v>
+      </c>
+      <c r="E9">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -656,13 +686,16 @@
       <c r="C10" s="1">
         <v>51229</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
+        <v>47428</v>
+      </c>
+      <c r="E10">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1">
         <v>37681</v>
@@ -670,13 +703,16 @@
       <c r="C11" s="1">
         <v>27877</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
+        <v>32047</v>
+      </c>
+      <c r="E11">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1">
         <v>33658</v>
@@ -684,11 +720,14 @@
       <c r="C12" s="1">
         <v>35279</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
+        <v>36132</v>
+      </c>
+      <c r="E12">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -698,13 +737,16 @@
       <c r="C13" s="1">
         <v>26491</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
+        <v>25870</v>
+      </c>
+      <c r="E13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1">
         <v>42253</v>
@@ -712,13 +754,16 @@
       <c r="C14" s="1">
         <v>41709</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
+        <v>34357</v>
+      </c>
+      <c r="E14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1">
         <v>26950</v>
@@ -726,13 +771,16 @@
       <c r="C15" s="1">
         <v>23300</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
+        <v>20100</v>
+      </c>
+      <c r="E15">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1">
         <v>25831</v>
@@ -740,11 +788,14 @@
       <c r="C16" s="1">
         <v>25850</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
+        <v>22765</v>
+      </c>
+      <c r="E16">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -754,11 +805,14 @@
       <c r="C17" s="1">
         <v>12360</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
+        <v>8826</v>
+      </c>
+      <c r="E17">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -768,11 +822,14 @@
       <c r="C18" s="1">
         <v>9915</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
+        <v>8986</v>
+      </c>
+      <c r="E18">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -782,13 +839,16 @@
       <c r="C19" s="1">
         <v>10490</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
+        <v>10617</v>
+      </c>
+      <c r="E19">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>6323</v>
@@ -796,13 +856,16 @@
       <c r="C20" s="1">
         <v>4733</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
+        <v>4086</v>
+      </c>
+      <c r="E20">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1">
         <v>3242</v>
@@ -810,11 +873,14 @@
       <c r="C21" s="1">
         <v>2865</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
+        <v>2797</v>
+      </c>
+      <c r="E21">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -824,11 +890,14 @@
       <c r="C22" s="1">
         <v>3311</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
+        <v>3462</v>
+      </c>
+      <c r="E22">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -838,13 +907,16 @@
       <c r="C23" s="1">
         <v>1481</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
+        <v>2095</v>
+      </c>
+      <c r="E23">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B24" s="1">
         <v>212415</v>
@@ -852,13 +924,16 @@
       <c r="C24" s="1">
         <v>245108</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
+        <v>248677</v>
+      </c>
+      <c r="E24">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B25" s="1">
         <v>205523</v>
@@ -867,10 +942,13 @@
         <v>207857</v>
       </c>
       <c r="D25">
+        <v>190423</v>
+      </c>
+      <c r="E25">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -881,12 +959,15 @@
         <v>188718</v>
       </c>
       <c r="D26">
+        <v>195255</v>
+      </c>
+      <c r="E26">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B27" s="1">
         <v>137913</v>
@@ -894,11 +975,14 @@
       <c r="C27" s="1">
         <v>174324</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
+        <v>181310</v>
+      </c>
+      <c r="E27">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -908,13 +992,16 @@
       <c r="C28" s="1">
         <v>133952</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
+        <v>120534</v>
+      </c>
+      <c r="E28">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B29" s="1">
         <v>72816</v>
@@ -922,11 +1009,14 @@
       <c r="C29" s="1">
         <v>92947</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
+        <v>110513</v>
+      </c>
+      <c r="E29">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -936,11 +1026,14 @@
       <c r="C30" s="1">
         <v>62768</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
+        <v>57499</v>
+      </c>
+      <c r="E30">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -950,11 +1043,14 @@
       <c r="C31" s="1">
         <v>56893</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
+        <v>56782</v>
+      </c>
+      <c r="E31">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -964,13 +1060,16 @@
       <c r="C32" s="1">
         <v>50504</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
+        <v>45101</v>
+      </c>
+      <c r="E32">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B33" s="1">
         <v>29580</v>
@@ -978,13 +1077,16 @@
       <c r="C33" s="1">
         <v>37263</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
+        <v>32879</v>
+      </c>
+      <c r="E33">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B34" s="1">
         <v>28420</v>
@@ -992,13 +1094,16 @@
       <c r="C34" s="1">
         <v>30257</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
+        <v>28330</v>
+      </c>
+      <c r="E34">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B35" s="1">
         <v>27455</v>
@@ -1006,11 +1111,14 @@
       <c r="C35" s="1">
         <v>29218</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
+        <v>26789</v>
+      </c>
+      <c r="E35">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1020,13 +1128,16 @@
       <c r="C36" s="1">
         <v>24374</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
+        <v>20660</v>
+      </c>
+      <c r="E36">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B37" s="1">
         <v>21650</v>
@@ -1035,12 +1146,15 @@
         <v>16450</v>
       </c>
       <c r="D37">
+        <v>16800</v>
+      </c>
+      <c r="E37">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B38" s="1">
         <v>19165</v>
@@ -1049,10 +1163,13 @@
         <v>20618</v>
       </c>
       <c r="D38">
+        <v>17082</v>
+      </c>
+      <c r="E38">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -1063,10 +1180,13 @@
         <v>9635</v>
       </c>
       <c r="D39">
+        <v>8181</v>
+      </c>
+      <c r="E39">
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1077,10 +1197,13 @@
         <v>9514</v>
       </c>
       <c r="D40">
+        <v>8547</v>
+      </c>
+      <c r="E40">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -1090,13 +1213,16 @@
       <c r="C41" s="1">
         <v>8188</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="1">
+        <v>7688</v>
+      </c>
+      <c r="E41">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B42" s="1">
         <v>4346</v>
@@ -1104,13 +1230,16 @@
       <c r="C42" s="1">
         <v>6326</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
+        <v>5673</v>
+      </c>
+      <c r="E42">
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B43" s="1">
         <v>2462</v>
@@ -1118,11 +1247,14 @@
       <c r="C43" s="1">
         <v>2881</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="1">
+        <v>3528</v>
+      </c>
+      <c r="E43">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -1132,11 +1264,14 @@
       <c r="C44" s="1">
         <v>2958</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="1">
+        <v>3197</v>
+      </c>
+      <c r="E44">
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -1146,13 +1281,16 @@
       <c r="C45" s="1">
         <v>1619</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="1">
+        <v>1529</v>
+      </c>
+      <c r="E45">
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B46" s="1">
         <v>259493</v>
@@ -1160,13 +1298,16 @@
       <c r="C46" s="1">
         <v>209870</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="1">
+        <v>238953</v>
+      </c>
+      <c r="E46">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B47" s="1">
         <v>203936</v>
@@ -1175,10 +1316,13 @@
         <v>188817</v>
       </c>
       <c r="D47">
+        <v>191102</v>
+      </c>
+      <c r="E47">
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -1189,12 +1333,15 @@
         <v>193571</v>
       </c>
       <c r="D48">
+        <v>191682</v>
+      </c>
+      <c r="E48">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B49" s="1">
         <v>159147</v>
@@ -1202,11 +1349,14 @@
       <c r="C49" s="1">
         <v>177120</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="1">
+        <v>177391</v>
+      </c>
+      <c r="E49">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>1</v>
       </c>
@@ -1216,13 +1366,16 @@
       <c r="C50" s="1">
         <v>131443</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="1">
+        <v>122182</v>
+      </c>
+      <c r="E50">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B51" s="1">
         <v>71679</v>
@@ -1230,11 +1383,14 @@
       <c r="C51" s="1">
         <v>103563</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="1">
+        <v>109962</v>
+      </c>
+      <c r="E51">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -1244,11 +1400,14 @@
       <c r="C52" s="1">
         <v>55531</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="1">
+        <v>55394</v>
+      </c>
+      <c r="E52">
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -1258,11 +1417,14 @@
       <c r="C53" s="1">
         <v>59029</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="1">
+        <v>53025</v>
+      </c>
+      <c r="E53">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -1272,13 +1434,16 @@
       <c r="C54" s="1">
         <v>50007</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="1">
+        <v>45102</v>
+      </c>
+      <c r="E54">
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B55" s="1">
         <v>29194</v>
@@ -1287,12 +1452,15 @@
         <v>28072</v>
       </c>
       <c r="D55">
+        <v>29000</v>
+      </c>
+      <c r="E55">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B56" s="1">
         <v>29082</v>
@@ -1301,12 +1469,15 @@
         <v>32130</v>
       </c>
       <c r="D56">
+        <v>31719</v>
+      </c>
+      <c r="E56">
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B57" s="1">
         <v>28077</v>
@@ -1314,11 +1485,14 @@
       <c r="C57" s="1">
         <v>28831</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="1">
+        <v>23262</v>
+      </c>
+      <c r="E57">
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -1329,12 +1503,15 @@
         <v>19520</v>
       </c>
       <c r="D58">
+        <v>18673</v>
+      </c>
+      <c r="E58">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B59" s="1">
         <v>19600</v>
@@ -1343,12 +1520,15 @@
         <v>14000</v>
       </c>
       <c r="D59">
+        <v>14800</v>
+      </c>
+      <c r="E59">
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B60" s="1">
         <v>17521</v>
@@ -1357,10 +1537,13 @@
         <v>19172</v>
       </c>
       <c r="D60">
+        <v>18970</v>
+      </c>
+      <c r="E60">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -1371,10 +1554,13 @@
         <v>8807</v>
       </c>
       <c r="D61">
+        <v>7327</v>
+      </c>
+      <c r="E61">
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -1384,11 +1570,14 @@
       <c r="C62" s="1">
         <v>8093</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="1">
+        <v>7846</v>
+      </c>
+      <c r="E62">
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>9</v>
       </c>
@@ -1399,12 +1588,15 @@
         <v>7372</v>
       </c>
       <c r="D63">
+        <v>8002</v>
+      </c>
+      <c r="E63">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B64" s="1">
         <v>4509</v>
@@ -1412,13 +1604,16 @@
       <c r="C64" s="1">
         <v>5447</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="1">
+        <v>4817</v>
+      </c>
+      <c r="E64">
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B65" s="1">
         <v>2845</v>
@@ -1426,11 +1621,14 @@
       <c r="C65" s="1">
         <v>3118</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="1">
+        <v>3166</v>
+      </c>
+      <c r="E65">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>11</v>
       </c>
@@ -1440,11 +1638,14 @@
       <c r="C66" s="1">
         <v>2350</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="1">
+        <v>2648</v>
+      </c>
+      <c r="E66">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -1454,13 +1655,16 @@
       <c r="C67" s="1">
         <v>1556</v>
       </c>
-      <c r="D67">
+      <c r="D67" s="1">
+        <v>1642</v>
+      </c>
+      <c r="E67">
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B68" s="1">
         <v>238542</v>
@@ -1468,13 +1672,16 @@
       <c r="C68" s="1">
         <v>209658</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="1">
+        <v>234043</v>
+      </c>
+      <c r="E68">
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B69" s="1">
         <v>199126</v>
@@ -1482,11 +1689,14 @@
       <c r="C69" s="1">
         <v>169656</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="1">
+        <v>203098</v>
+      </c>
+      <c r="E69">
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -1497,12 +1707,15 @@
         <v>173333</v>
       </c>
       <c r="D70">
+        <v>196496</v>
+      </c>
+      <c r="E70">
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B71" s="1">
         <v>178807</v>
@@ -1511,10 +1724,13 @@
         <v>181221</v>
       </c>
       <c r="D71">
+        <v>199819</v>
+      </c>
+      <c r="E71">
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>1</v>
       </c>
@@ -1524,13 +1740,16 @@
       <c r="C72" s="1">
         <v>113925</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="1">
+        <v>132668</v>
+      </c>
+      <c r="E72">
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B73" s="1">
         <v>73854</v>
@@ -1538,11 +1757,14 @@
       <c r="C73" s="1">
         <v>101244</v>
       </c>
-      <c r="D73">
+      <c r="D73" s="1">
+        <v>122819</v>
+      </c>
+      <c r="E73">
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>3</v>
       </c>
@@ -1553,10 +1775,13 @@
         <v>51659</v>
       </c>
       <c r="D74">
+        <v>57044</v>
+      </c>
+      <c r="E74">
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>2</v>
       </c>
@@ -1567,10 +1792,13 @@
         <v>53510</v>
       </c>
       <c r="D75">
+        <v>57359</v>
+      </c>
+      <c r="E75">
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>4</v>
       </c>
@@ -1580,13 +1808,16 @@
       <c r="C76" s="1">
         <v>44619</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="1">
+        <v>51503</v>
+      </c>
+      <c r="E76">
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B77" s="1">
         <v>28750</v>
@@ -1595,12 +1826,15 @@
         <v>26947</v>
       </c>
       <c r="D77">
+        <v>30555</v>
+      </c>
+      <c r="E77">
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B78" s="1">
         <v>27964</v>
@@ -1609,10 +1843,13 @@
         <v>27442</v>
       </c>
       <c r="D78">
+        <v>25908</v>
+      </c>
+      <c r="E78">
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -1623,12 +1860,15 @@
         <v>18838</v>
       </c>
       <c r="D79">
+        <v>21257</v>
+      </c>
+      <c r="E79">
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B80" s="1">
         <v>22052</v>
@@ -1637,12 +1877,15 @@
         <v>32003</v>
       </c>
       <c r="D80">
+        <v>30617</v>
+      </c>
+      <c r="E80">
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B81" s="1">
         <v>20900</v>
@@ -1650,13 +1893,16 @@
       <c r="C81" s="1">
         <v>16000</v>
       </c>
-      <c r="D81">
+      <c r="D81" s="1">
+        <v>19319</v>
+      </c>
+      <c r="E81">
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B82" s="1">
         <v>16356</v>
@@ -1664,11 +1910,14 @@
       <c r="C82" s="1">
         <v>16130</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="1">
+        <v>14100</v>
+      </c>
+      <c r="E82">
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>6</v>
       </c>
@@ -1678,11 +1927,14 @@
       <c r="C83" s="1">
         <v>9323</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="1">
+        <v>8715</v>
+      </c>
+      <c r="E83">
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>10</v>
       </c>
@@ -1693,10 +1945,13 @@
         <v>7488</v>
       </c>
       <c r="D84">
+        <v>6966</v>
+      </c>
+      <c r="E84">
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>9</v>
       </c>
@@ -1707,12 +1962,15 @@
         <v>7722</v>
       </c>
       <c r="D85">
+        <v>7705</v>
+      </c>
+      <c r="E85">
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B86" s="1">
         <v>5008</v>
@@ -1720,13 +1978,16 @@
       <c r="C86" s="1">
         <v>5213</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="1">
+        <v>5102</v>
+      </c>
+      <c r="E86">
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B87" s="1">
         <v>2947</v>
@@ -1734,11 +1995,14 @@
       <c r="C87" s="1">
         <v>3498</v>
       </c>
-      <c r="D87">
+      <c r="D87" s="1">
+        <v>3461</v>
+      </c>
+      <c r="E87">
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>11</v>
       </c>
@@ -1748,11 +2012,14 @@
       <c r="C88" s="1">
         <v>2002</v>
       </c>
-      <c r="D88">
+      <c r="D88" s="1">
+        <v>2040</v>
+      </c>
+      <c r="E88">
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>7</v>
       </c>
@@ -1762,13 +2029,16 @@
       <c r="C89" s="1">
         <v>1264</v>
       </c>
-      <c r="D89">
+      <c r="D89" s="1">
+        <v>1377</v>
+      </c>
+      <c r="E89">
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B90" s="1">
         <v>218845</v>
@@ -1777,12 +2047,15 @@
         <v>289475</v>
       </c>
       <c r="D90" s="1">
+        <v>238574</v>
+      </c>
+      <c r="E90" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B91" s="1">
         <v>190532</v>
@@ -1791,10 +2064,13 @@
         <v>248334</v>
       </c>
       <c r="D91" s="1">
+        <v>223055</v>
+      </c>
+      <c r="E91" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>0</v>
       </c>
@@ -1805,12 +2081,15 @@
         <v>209953</v>
       </c>
       <c r="D92" s="1">
+        <v>217700</v>
+      </c>
+      <c r="E92" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B93" s="1">
         <v>171519</v>
@@ -1819,10 +2098,13 @@
         <v>215240</v>
       </c>
       <c r="D93" s="1">
+        <v>193718</v>
+      </c>
+      <c r="E93" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>1</v>
       </c>
@@ -1833,12 +2115,15 @@
         <v>173993</v>
       </c>
       <c r="D94" s="1">
+        <v>147903</v>
+      </c>
+      <c r="E94" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B95" s="1">
         <v>73833</v>
@@ -1847,10 +2132,13 @@
         <v>127230</v>
       </c>
       <c r="D95" s="1">
+        <v>112376</v>
+      </c>
+      <c r="E95" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>2</v>
       </c>
@@ -1861,10 +2149,13 @@
         <v>65494</v>
       </c>
       <c r="D96" s="1">
+        <v>57542</v>
+      </c>
+      <c r="E96" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>3</v>
       </c>
@@ -1875,10 +2166,13 @@
         <v>70039</v>
       </c>
       <c r="D97" s="1">
+        <v>64088</v>
+      </c>
+      <c r="E97" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>4</v>
       </c>
@@ -1889,12 +2183,15 @@
         <v>60730</v>
       </c>
       <c r="D98" s="1">
+        <v>53864</v>
+      </c>
+      <c r="E98" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B99" s="1">
         <v>29973</v>
@@ -1903,10 +2200,13 @@
         <v>35412</v>
       </c>
       <c r="D99" s="1">
+        <v>32255</v>
+      </c>
+      <c r="E99" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
         <v>5</v>
       </c>
@@ -1917,12 +2217,15 @@
         <v>27482</v>
       </c>
       <c r="D100" s="1">
+        <v>25816</v>
+      </c>
+      <c r="E100" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B101" s="1">
         <v>23966</v>
@@ -1931,12 +2234,15 @@
         <v>30144</v>
       </c>
       <c r="D101" s="1">
+        <v>24084</v>
+      </c>
+      <c r="E101" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B102" s="1">
         <v>21987</v>
@@ -1945,12 +2251,15 @@
         <v>29646</v>
       </c>
       <c r="D102" s="1">
+        <v>23789</v>
+      </c>
+      <c r="E102" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B103" s="1">
         <v>19000</v>
@@ -1959,12 +2268,15 @@
         <v>13200</v>
       </c>
       <c r="D103" s="1">
+        <v>20907</v>
+      </c>
+      <c r="E103" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B104" s="1">
         <v>15901</v>
@@ -1973,10 +2285,13 @@
         <v>21531</v>
       </c>
       <c r="D104" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E104" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:5">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -1987,12 +2302,15 @@
         <v>9194</v>
       </c>
       <c r="D105" s="1">
+        <v>8970</v>
+      </c>
+      <c r="E105" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B106" s="1">
         <v>7162</v>
@@ -2001,12 +2319,15 @@
         <v>8139</v>
       </c>
       <c r="D106" s="1">
+        <v>8416</v>
+      </c>
+      <c r="E106" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B107" s="1">
         <v>5184</v>
@@ -2015,12 +2336,15 @@
         <v>6572</v>
       </c>
       <c r="D107" s="1">
+        <v>7179</v>
+      </c>
+      <c r="E107" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B108" s="1">
         <v>4085</v>
@@ -2029,12 +2353,15 @@
         <v>4636</v>
       </c>
       <c r="D108" s="1">
+        <v>4083</v>
+      </c>
+      <c r="E108" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B109" s="1">
         <v>3133</v>
@@ -2043,10 +2370,13 @@
         <v>3927</v>
       </c>
       <c r="D109" s="1">
+        <v>3800</v>
+      </c>
+      <c r="E109" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:5">
       <c r="A110" t="s">
         <v>11</v>
       </c>
@@ -2057,10 +2387,13 @@
         <v>2128</v>
       </c>
       <c r="D110" s="1">
+        <v>2469</v>
+      </c>
+      <c r="E110" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:5">
       <c r="A111" t="s">
         <v>7</v>
       </c>
@@ -2071,12 +2404,15 @@
         <v>1326</v>
       </c>
       <c r="D111" s="1">
+        <v>1572</v>
+      </c>
+      <c r="E111" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B112" s="1">
         <v>204756</v>
@@ -2085,10 +2421,13 @@
         <v>236518</v>
       </c>
       <c r="D112" s="1">
+        <v>221437</v>
+      </c>
+      <c r="E112" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
         <v>0</v>
       </c>
@@ -2099,12 +2438,15 @@
         <v>192720</v>
       </c>
       <c r="D113" s="1">
+        <v>192743</v>
+      </c>
+      <c r="E113" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B114" s="1">
         <v>168791</v>
@@ -2113,12 +2455,15 @@
         <v>209204</v>
       </c>
       <c r="D114" s="1">
+        <v>208770</v>
+      </c>
+      <c r="E114" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B115" s="1">
         <v>157025</v>
@@ -2127,10 +2472,13 @@
         <v>168573</v>
       </c>
       <c r="D115" s="1">
+        <v>170970</v>
+      </c>
+      <c r="E115" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
         <v>1</v>
       </c>
@@ -2141,12 +2489,15 @@
         <v>141296</v>
       </c>
       <c r="D116" s="1">
+        <v>138602</v>
+      </c>
+      <c r="E116" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:5">
       <c r="A117" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B117" s="1">
         <v>73463</v>
@@ -2155,10 +2506,13 @@
         <v>98880</v>
       </c>
       <c r="D117" s="1">
+        <v>108792</v>
+      </c>
+      <c r="E117" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
         <v>2</v>
       </c>
@@ -2169,10 +2523,13 @@
         <v>58926</v>
       </c>
       <c r="D118" s="1">
+        <v>51752</v>
+      </c>
+      <c r="E118" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:5">
       <c r="A119" t="s">
         <v>4</v>
       </c>
@@ -2183,10 +2540,13 @@
         <v>53405</v>
       </c>
       <c r="D119" s="1">
+        <v>53112</v>
+      </c>
+      <c r="E119" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:5">
       <c r="A120" t="s">
         <v>3</v>
       </c>
@@ -2197,12 +2557,15 @@
         <v>64106</v>
       </c>
       <c r="D120" s="1">
+        <v>59426</v>
+      </c>
+      <c r="E120" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:5">
       <c r="A121" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B121" s="1">
         <v>27723</v>
@@ -2211,12 +2574,15 @@
         <v>31188</v>
       </c>
       <c r="D121" s="1">
+        <v>30520</v>
+      </c>
+      <c r="E121" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:5">
       <c r="A122" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B122" s="1">
         <v>26850</v>
@@ -2225,10 +2591,13 @@
         <v>27490</v>
       </c>
       <c r="D122" s="1">
+        <v>22955</v>
+      </c>
+      <c r="E122" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:5">
       <c r="A123" t="s">
         <v>5</v>
       </c>
@@ -2239,12 +2608,15 @@
         <v>23292</v>
       </c>
       <c r="D123" s="1">
+        <v>24125</v>
+      </c>
+      <c r="E123" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:5">
       <c r="A124" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B124" s="1">
         <v>19619</v>
@@ -2253,12 +2625,15 @@
         <v>25915</v>
       </c>
       <c r="D124" s="1">
+        <v>21982</v>
+      </c>
+      <c r="E124" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:5">
       <c r="A125" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B125" s="1">
         <v>15800</v>
@@ -2267,12 +2642,15 @@
         <v>12800</v>
       </c>
       <c r="D125" s="1">
+        <v>9300</v>
+      </c>
+      <c r="E125" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:5">
       <c r="A126" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B126" s="1">
         <v>15636</v>
@@ -2281,10 +2659,13 @@
         <v>19370</v>
       </c>
       <c r="D126" s="1">
+        <v>19221</v>
+      </c>
+      <c r="E126" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
         <v>6</v>
       </c>
@@ -2295,12 +2676,15 @@
         <v>8795</v>
       </c>
       <c r="D127" s="1">
+        <v>8622</v>
+      </c>
+      <c r="E127" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:5">
       <c r="A128" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B128" s="1">
         <v>5597</v>
@@ -2309,12 +2693,15 @@
         <v>8613</v>
       </c>
       <c r="D128" s="1">
+        <v>9950</v>
+      </c>
+      <c r="E128" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:5">
       <c r="A129" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B129" s="1">
         <v>5294</v>
@@ -2323,12 +2710,15 @@
         <v>6456</v>
       </c>
       <c r="D129" s="1">
+        <v>6209</v>
+      </c>
+      <c r="E129" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:5">
       <c r="A130" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B130" s="1">
         <v>4063</v>
@@ -2337,12 +2727,15 @@
         <v>4956</v>
       </c>
       <c r="D130" s="1">
+        <v>4020</v>
+      </c>
+      <c r="E130" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:5">
       <c r="A131" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B131" s="1">
         <v>2984</v>
@@ -2351,10 +2744,13 @@
         <v>2867</v>
       </c>
       <c r="D131" s="1">
+        <v>4296</v>
+      </c>
+      <c r="E131" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:5">
       <c r="A132" t="s">
         <v>11</v>
       </c>
@@ -2365,10 +2761,13 @@
         <v>2020</v>
       </c>
       <c r="D132" s="1">
+        <v>1880</v>
+      </c>
+      <c r="E132" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:5">
       <c r="A133" t="s">
         <v>7</v>
       </c>
@@ -2379,12 +2778,15 @@
         <v>1310</v>
       </c>
       <c r="D133" s="1">
+        <v>1618</v>
+      </c>
+      <c r="E133" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:5">
       <c r="A134" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B134" s="1">
         <v>175770</v>
@@ -2393,10 +2795,13 @@
         <v>249182</v>
       </c>
       <c r="D134" s="1">
+        <v>279856</v>
+      </c>
+      <c r="E134" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:5">
       <c r="A135" t="s">
         <v>0</v>
       </c>
@@ -2407,12 +2812,15 @@
         <v>218691</v>
       </c>
       <c r="D135" s="1">
+        <v>229537</v>
+      </c>
+      <c r="E135" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:5">
       <c r="A136" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B136" s="1">
         <v>149445</v>
@@ -2421,12 +2829,15 @@
         <v>202352</v>
       </c>
       <c r="D136" s="1">
+        <v>209602</v>
+      </c>
+      <c r="E136" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:5">
       <c r="A137" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B137" s="1">
         <v>137902</v>
@@ -2435,10 +2846,13 @@
         <v>206083</v>
       </c>
       <c r="D137" s="1">
+        <v>202264</v>
+      </c>
+      <c r="E137" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:5">
       <c r="A138" t="s">
         <v>1</v>
       </c>
@@ -2449,12 +2863,15 @@
         <v>135901</v>
       </c>
       <c r="D138" s="1">
+        <v>146563</v>
+      </c>
+      <c r="E138" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:5">
       <c r="A139" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B139" s="1">
         <v>65290</v>
@@ -2463,10 +2880,13 @@
         <v>123504</v>
       </c>
       <c r="D139" s="1">
+        <v>145096</v>
+      </c>
+      <c r="E139" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:5">
       <c r="A140" t="s">
         <v>3</v>
       </c>
@@ -2477,10 +2897,13 @@
         <v>61511</v>
       </c>
       <c r="D140" s="1">
+        <v>59841</v>
+      </c>
+      <c r="E140" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:5">
       <c r="A141" t="s">
         <v>2</v>
       </c>
@@ -2491,10 +2914,13 @@
         <v>66089</v>
       </c>
       <c r="D141" s="1">
+        <v>64052</v>
+      </c>
+      <c r="E141" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:5">
       <c r="A142" t="s">
         <v>4</v>
       </c>
@@ -2505,10 +2931,13 @@
         <v>56801</v>
       </c>
       <c r="D142" s="1">
+        <v>56571</v>
+      </c>
+      <c r="E142" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:5">
       <c r="A143" t="s">
         <v>5</v>
       </c>
@@ -2519,12 +2948,15 @@
         <v>22828</v>
       </c>
       <c r="D143" s="1">
+        <v>26893</v>
+      </c>
+      <c r="E143" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:5">
       <c r="A144" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B144" s="1">
         <v>24945</v>
@@ -2533,12 +2965,15 @@
         <v>31725</v>
       </c>
       <c r="D144" s="1">
+        <v>28941</v>
+      </c>
+      <c r="E144" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:5">
       <c r="A145" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B145" s="1">
         <v>24528</v>
@@ -2547,12 +2982,15 @@
         <v>29201</v>
       </c>
       <c r="D145" s="1">
+        <v>28999</v>
+      </c>
+      <c r="E145" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:5">
       <c r="A146" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B146" s="1">
         <v>22488</v>
@@ -2561,12 +2999,15 @@
         <v>31474</v>
       </c>
       <c r="D146" s="1">
+        <v>29407</v>
+      </c>
+      <c r="E146" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:5">
       <c r="A147" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B147" s="1">
         <v>15218</v>
@@ -2575,12 +3016,15 @@
         <v>19409</v>
       </c>
       <c r="D147" s="1">
+        <v>19471</v>
+      </c>
+      <c r="E147" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:5">
       <c r="A148" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B148" s="1">
         <v>11150</v>
@@ -2589,10 +3033,13 @@
         <v>14400</v>
       </c>
       <c r="D148" s="1">
+        <v>8200</v>
+      </c>
+      <c r="E148" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:5">
       <c r="A149" t="s">
         <v>6</v>
       </c>
@@ -2603,12 +3050,15 @@
         <v>9934</v>
       </c>
       <c r="D149" s="1">
+        <v>9869</v>
+      </c>
+      <c r="E149" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:5">
       <c r="A150" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B150" s="1">
         <v>6576</v>
@@ -2617,12 +3067,15 @@
         <v>6593</v>
       </c>
       <c r="D150" s="1">
+        <v>6982</v>
+      </c>
+      <c r="E150" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:5">
       <c r="A151" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B151" s="1">
         <v>5382</v>
@@ -2631,10 +3084,13 @@
         <v>5205</v>
       </c>
       <c r="D151" s="1">
+        <v>4892</v>
+      </c>
+      <c r="E151" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:5">
       <c r="A152" t="s">
         <v>9</v>
       </c>
@@ -2645,12 +3101,15 @@
         <v>12317</v>
       </c>
       <c r="D152" s="1">
+        <v>11149</v>
+      </c>
+      <c r="E152" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:5">
       <c r="A153" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B153" s="1">
         <v>2333</v>
@@ -2659,10 +3118,13 @@
         <v>3304</v>
       </c>
       <c r="D153" s="1">
+        <v>4146</v>
+      </c>
+      <c r="E153" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:5">
       <c r="A154" t="s">
         <v>11</v>
       </c>
@@ -2673,10 +3135,13 @@
         <v>1892</v>
       </c>
       <c r="D154" s="1">
+        <v>2353</v>
+      </c>
+      <c r="E154" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:5">
       <c r="A155" t="s">
         <v>7</v>
       </c>
@@ -2687,12 +3152,15 @@
         <v>1409</v>
       </c>
       <c r="D155" s="1">
+        <v>1754</v>
+      </c>
+      <c r="E155" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:5">
       <c r="A156" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B156" s="1">
         <v>175921</v>
@@ -2700,13 +3168,16 @@
       <c r="C156" s="1">
         <v>261452</v>
       </c>
-      <c r="D156" s="1">
+      <c r="D156">
+        <v>254895</v>
+      </c>
+      <c r="E156" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:5">
       <c r="A157" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B157" s="1">
         <v>163421</v>
@@ -2715,10 +3186,13 @@
         <v>222174</v>
       </c>
       <c r="D157" s="1">
+        <v>215321</v>
+      </c>
+      <c r="E157" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:5">
       <c r="A158" t="s">
         <v>0</v>
       </c>
@@ -2729,12 +3203,15 @@
         <v>231588</v>
       </c>
       <c r="D158" s="1">
+        <v>241527</v>
+      </c>
+      <c r="E158" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:5">
       <c r="A159" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B159" s="1">
         <v>137119</v>
@@ -2743,10 +3220,13 @@
         <v>218702</v>
       </c>
       <c r="D159" s="1">
+        <v>214294</v>
+      </c>
+      <c r="E159" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:5">
       <c r="A160" t="s">
         <v>1</v>
       </c>
@@ -2757,12 +3237,15 @@
         <v>145532</v>
       </c>
       <c r="D160" s="1">
+        <v>153069</v>
+      </c>
+      <c r="E160" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:5">
       <c r="A161" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B161" s="1">
         <v>65349</v>
@@ -2771,10 +3254,13 @@
         <v>131983</v>
       </c>
       <c r="D161" s="1">
+        <v>131832</v>
+      </c>
+      <c r="E161" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="1:4">
+    <row r="162" spans="1:5">
       <c r="A162" t="s">
         <v>2</v>
       </c>
@@ -2785,10 +3271,13 @@
         <v>68434</v>
       </c>
       <c r="D162" s="1">
+        <v>66056</v>
+      </c>
+      <c r="E162" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="1:4">
+    <row r="163" spans="1:5">
       <c r="A163" t="s">
         <v>3</v>
       </c>
@@ -2799,10 +3288,13 @@
         <v>63972</v>
       </c>
       <c r="D163" s="1">
+        <v>60146</v>
+      </c>
+      <c r="E163" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="1:4">
+    <row r="164" spans="1:5">
       <c r="A164" t="s">
         <v>4</v>
       </c>
@@ -2813,12 +3305,15 @@
         <v>60062</v>
       </c>
       <c r="D164" s="1">
+        <v>59462</v>
+      </c>
+      <c r="E164" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="1:4">
+    <row r="165" spans="1:5">
       <c r="A165" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B165" s="1">
         <v>24944</v>
@@ -2827,10 +3322,13 @@
         <v>35702</v>
       </c>
       <c r="D165" s="1">
+        <v>31211</v>
+      </c>
+      <c r="E165" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="1:4">
+    <row r="166" spans="1:5">
       <c r="A166" t="s">
         <v>5</v>
       </c>
@@ -2841,12 +3339,15 @@
         <v>25192</v>
       </c>
       <c r="D166" s="1">
+        <v>29980</v>
+      </c>
+      <c r="E166" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:4">
+    <row r="167" spans="1:5">
       <c r="A167" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B167" s="1">
         <v>20958</v>
@@ -2855,12 +3356,15 @@
         <v>29942</v>
       </c>
       <c r="D167" s="1">
+        <v>30077</v>
+      </c>
+      <c r="E167" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:4">
+    <row r="168" spans="1:5">
       <c r="A168" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B168" s="1">
         <v>18075</v>
@@ -2869,12 +3373,15 @@
         <v>27707</v>
       </c>
       <c r="D168" s="1">
+        <v>26662</v>
+      </c>
+      <c r="E168" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="1:4">
+    <row r="169" spans="1:5">
       <c r="A169" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B169" s="1">
         <v>13487</v>
@@ -2883,10 +3390,13 @@
         <v>18892</v>
       </c>
       <c r="D169" s="1">
+        <v>19315</v>
+      </c>
+      <c r="E169" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="1:4">
+    <row r="170" spans="1:5">
       <c r="A170" t="s">
         <v>6</v>
       </c>
@@ -2897,12 +3407,15 @@
         <v>9761</v>
       </c>
       <c r="D170" s="1">
+        <v>9338</v>
+      </c>
+      <c r="E170" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:4">
+    <row r="171" spans="1:5">
       <c r="A171" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B171" s="1">
         <v>8150</v>
@@ -2911,12 +3424,15 @@
         <v>11300</v>
       </c>
       <c r="D171" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E171" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="1:4">
+    <row r="172" spans="1:5">
       <c r="A172" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B172" s="1">
         <v>5136</v>
@@ -2925,10 +3441,13 @@
         <v>7337</v>
       </c>
       <c r="D172" s="1">
+        <v>7103</v>
+      </c>
+      <c r="E172" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:4">
+    <row r="173" spans="1:5">
       <c r="A173" t="s">
         <v>9</v>
       </c>
@@ -2939,12 +3458,15 @@
         <v>9750</v>
       </c>
       <c r="D173" s="1">
+        <v>12416</v>
+      </c>
+      <c r="E173" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:4">
+    <row r="174" spans="1:5">
       <c r="A174" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B174" s="1">
         <v>3506</v>
@@ -2953,12 +3475,15 @@
         <v>5010</v>
       </c>
       <c r="D174" s="1">
+        <v>5005</v>
+      </c>
+      <c r="E174" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:4">
+    <row r="175" spans="1:5">
       <c r="A175" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B175" s="1">
         <v>1909</v>
@@ -2967,10 +3492,13 @@
         <v>2964</v>
       </c>
       <c r="D175" s="1">
+        <v>4226</v>
+      </c>
+      <c r="E175" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:5">
       <c r="A176" t="s">
         <v>11</v>
       </c>
@@ -2981,10 +3509,13 @@
         <v>2021</v>
       </c>
       <c r="D176" s="1">
+        <v>2366</v>
+      </c>
+      <c r="E176" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:4">
+    <row r="177" spans="1:5">
       <c r="A177" t="s">
         <v>7</v>
       </c>
@@ -2995,12 +3526,15 @@
         <v>1374</v>
       </c>
       <c r="D177" s="1">
+        <v>1705</v>
+      </c>
+      <c r="E177" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="178" spans="1:4">
+    <row r="178" spans="1:5">
       <c r="A178" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B178" s="1">
         <v>137573</v>
@@ -3008,11 +3542,14 @@
       <c r="C178" s="1">
         <v>233682</v>
       </c>
-      <c r="D178" s="1">
+      <c r="D178">
+        <v>236116</v>
+      </c>
+      <c r="E178" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="1:4">
+    <row r="179" spans="1:5">
       <c r="A179" t="s">
         <v>0</v>
       </c>
@@ -3023,12 +3560,15 @@
         <v>194219</v>
       </c>
       <c r="D179" s="1">
+        <v>203856</v>
+      </c>
+      <c r="E179" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:4">
+    <row r="180" spans="1:5">
       <c r="A180" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B180" s="1">
         <v>92053</v>
@@ -3037,12 +3577,15 @@
         <v>172900</v>
       </c>
       <c r="D180" s="1">
+        <v>184149</v>
+      </c>
+      <c r="E180" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:4">
+    <row r="181" spans="1:5">
       <c r="A181" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B181" s="1">
         <v>85163</v>
@@ -3051,10 +3594,13 @@
         <v>183866</v>
       </c>
       <c r="D181" s="1">
+        <v>192348</v>
+      </c>
+      <c r="E181" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:4">
+    <row r="182" spans="1:5">
       <c r="A182" t="s">
         <v>1</v>
       </c>
@@ -3065,12 +3611,15 @@
         <v>125775</v>
       </c>
       <c r="D182" s="1">
+        <v>125701</v>
+      </c>
+      <c r="E182" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="183" spans="1:4">
+    <row r="183" spans="1:5">
       <c r="A183" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B183" s="1">
         <v>46689</v>
@@ -3079,10 +3628,13 @@
         <v>95698</v>
       </c>
       <c r="D183" s="1">
+        <v>87764</v>
+      </c>
+      <c r="E183" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:4">
+    <row r="184" spans="1:5">
       <c r="A184" t="s">
         <v>2</v>
       </c>
@@ -3093,10 +3645,13 @@
         <v>57025</v>
       </c>
       <c r="D184" s="1">
+        <v>56063</v>
+      </c>
+      <c r="E184" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:4">
+    <row r="185" spans="1:5">
       <c r="A185" t="s">
         <v>4</v>
       </c>
@@ -3107,10 +3662,13 @@
         <v>51385</v>
       </c>
       <c r="D185" s="1">
+        <v>50585</v>
+      </c>
+      <c r="E185" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="186" spans="1:4">
+    <row r="186" spans="1:5">
       <c r="A186" t="s">
         <v>3</v>
       </c>
@@ -3121,12 +3679,15 @@
         <v>57288</v>
       </c>
       <c r="D186" s="1">
+        <v>53170</v>
+      </c>
+      <c r="E186" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="187" spans="1:4">
+    <row r="187" spans="1:5">
       <c r="A187" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B187" s="1">
         <v>20043</v>
@@ -3135,12 +3696,15 @@
         <v>31309</v>
       </c>
       <c r="D187" s="1">
+        <v>28794</v>
+      </c>
+      <c r="E187" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:4">
+    <row r="188" spans="1:5">
       <c r="A188" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B188" s="1">
         <v>11278</v>
@@ -3149,10 +3713,13 @@
         <v>25631</v>
       </c>
       <c r="D188" s="1">
+        <v>30022</v>
+      </c>
+      <c r="E188" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="189" spans="1:4">
+    <row r="189" spans="1:5">
       <c r="A189" t="s">
         <v>5</v>
       </c>
@@ -3163,12 +3730,15 @@
         <v>19702</v>
       </c>
       <c r="D189" s="1">
+        <v>23056</v>
+      </c>
+      <c r="E189" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="190" spans="1:4">
+    <row r="190" spans="1:5">
       <c r="A190" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B190" s="1">
         <v>7233</v>
@@ -3177,12 +3747,15 @@
         <v>23816</v>
       </c>
       <c r="D190" s="1">
+        <v>23482</v>
+      </c>
+      <c r="E190" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="191" spans="1:4">
+    <row r="191" spans="1:5">
       <c r="A191" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B191" s="1">
         <v>6200</v>
@@ -3191,12 +3764,15 @@
         <v>10600</v>
       </c>
       <c r="D191" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E191" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:4">
+    <row r="192" spans="1:5">
       <c r="A192" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B192" s="1">
         <v>6138</v>
@@ -3205,10 +3781,13 @@
         <v>15024</v>
       </c>
       <c r="D192" s="1">
+        <v>19104</v>
+      </c>
+      <c r="E192" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:4">
+    <row r="193" spans="1:5">
       <c r="A193" t="s">
         <v>6</v>
       </c>
@@ -3219,12 +3798,15 @@
         <v>8367</v>
       </c>
       <c r="D193" s="1">
+        <v>8333</v>
+      </c>
+      <c r="E193" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:4">
+    <row r="194" spans="1:5">
       <c r="A194" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B194" s="1">
         <v>2865</v>
@@ -3233,10 +3815,13 @@
         <v>7165</v>
       </c>
       <c r="D194" s="1">
+        <v>6448</v>
+      </c>
+      <c r="E194" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:4">
+    <row r="195" spans="1:5">
       <c r="A195" t="s">
         <v>9</v>
       </c>
@@ -3247,12 +3832,15 @@
         <v>6963</v>
       </c>
       <c r="D195" s="1">
+        <v>7990</v>
+      </c>
+      <c r="E195" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="196" spans="1:4">
+    <row r="196" spans="1:5">
       <c r="A196" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B196" s="1">
         <v>2007</v>
@@ -3261,12 +3849,15 @@
         <v>5018</v>
       </c>
       <c r="D196" s="1">
+        <v>5570</v>
+      </c>
+      <c r="E196" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:4">
+    <row r="197" spans="1:5">
       <c r="A197" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B197">
         <v>991</v>
@@ -3275,10 +3866,13 @@
         <v>2621</v>
       </c>
       <c r="D197" s="1">
+        <v>3731</v>
+      </c>
+      <c r="E197" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:4">
+    <row r="198" spans="1:5">
       <c r="A198" t="s">
         <v>11</v>
       </c>
@@ -3289,10 +3883,13 @@
         <v>2147</v>
       </c>
       <c r="D198" s="1">
+        <v>2019</v>
+      </c>
+      <c r="E198" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:4">
+    <row r="199" spans="1:5">
       <c r="A199" t="s">
         <v>7</v>
       </c>
@@ -3303,12 +3900,15 @@
         <v>1385</v>
       </c>
       <c r="D199" s="1">
+        <v>1593</v>
+      </c>
+      <c r="E199" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:4">
+    <row r="200" spans="1:5">
       <c r="A200" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B200" s="1">
         <v>169952</v>
@@ -3317,10 +3917,13 @@
         <v>271205</v>
       </c>
       <c r="D200" s="1">
+        <v>296138</v>
+      </c>
+      <c r="E200" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="201" spans="1:4">
+    <row r="201" spans="1:5">
       <c r="A201" t="s">
         <v>0</v>
       </c>
@@ -3331,12 +3934,15 @@
         <v>230382</v>
       </c>
       <c r="D201" s="1">
+        <v>243021</v>
+      </c>
+      <c r="E201" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="1:4">
+    <row r="202" spans="1:5">
       <c r="A202" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B202" s="1">
         <v>133198</v>
@@ -3345,12 +3951,15 @@
         <v>214947</v>
       </c>
       <c r="D202" s="1">
+        <v>222782</v>
+      </c>
+      <c r="E202" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="203" spans="1:4">
+    <row r="203" spans="1:5">
       <c r="A203" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B203" s="1">
         <v>127596</v>
@@ -3359,12 +3968,15 @@
         <v>200307</v>
       </c>
       <c r="D203" s="1">
+        <v>216063</v>
+      </c>
+      <c r="E203" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="204" spans="1:4">
+    <row r="204" spans="1:5">
       <c r="A204" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B204" s="1">
         <v>77655</v>
@@ -3373,10 +3985,13 @@
         <v>150768</v>
       </c>
       <c r="D204" s="1">
+        <v>162535</v>
+      </c>
+      <c r="E204" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="205" spans="1:4">
+    <row r="205" spans="1:5">
       <c r="A205" t="s">
         <v>1</v>
       </c>
@@ -3387,10 +4002,13 @@
         <v>148509</v>
       </c>
       <c r="D205" s="1">
+        <v>142392</v>
+      </c>
+      <c r="E205" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="206" spans="1:4">
+    <row r="206" spans="1:5">
       <c r="A206" t="s">
         <v>4</v>
       </c>
@@ -3401,10 +4019,13 @@
         <v>55814</v>
       </c>
       <c r="D206" s="1">
+        <v>50645</v>
+      </c>
+      <c r="E206" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="207" spans="1:4">
+    <row r="207" spans="1:5">
       <c r="A207" t="s">
         <v>2</v>
       </c>
@@ -3415,10 +4036,13 @@
         <v>62627</v>
       </c>
       <c r="D207" s="1">
+        <v>61540</v>
+      </c>
+      <c r="E207" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="208" spans="1:4">
+    <row r="208" spans="1:5">
       <c r="A208" t="s">
         <v>3</v>
       </c>
@@ -3429,12 +4053,15 @@
         <v>61601</v>
       </c>
       <c r="D208" s="1">
+        <v>58097</v>
+      </c>
+      <c r="E208" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="209" spans="1:4">
+    <row r="209" spans="1:5">
       <c r="A209" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B209" s="1">
         <v>21620</v>
@@ -3443,12 +4070,15 @@
         <v>37092</v>
       </c>
       <c r="D209" s="1">
+        <v>32548</v>
+      </c>
+      <c r="E209" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="210" spans="1:4">
+    <row r="210" spans="1:5">
       <c r="A210" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B210" s="1">
         <v>18571</v>
@@ -3457,12 +4087,15 @@
         <v>30537</v>
       </c>
       <c r="D210" s="1">
+        <v>31374</v>
+      </c>
+      <c r="E210" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="211" spans="1:4">
+    <row r="211" spans="1:5">
       <c r="A211" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B211" s="1">
         <v>16006</v>
@@ -3471,10 +4104,13 @@
         <v>32228</v>
       </c>
       <c r="D211" s="1">
+        <v>31311</v>
+      </c>
+      <c r="E211" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="212" spans="1:4">
+    <row r="212" spans="1:5">
       <c r="A212" t="s">
         <v>5</v>
       </c>
@@ -3485,12 +4121,15 @@
         <v>26934</v>
       </c>
       <c r="D212" s="1">
+        <v>33302</v>
+      </c>
+      <c r="E212" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="213" spans="1:4">
+    <row r="213" spans="1:5">
       <c r="A213" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B213" s="1">
         <v>13400</v>
@@ -3499,12 +4138,15 @@
         <v>13000</v>
       </c>
       <c r="D213" s="1">
+        <v>4050</v>
+      </c>
+      <c r="E213" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="214" spans="1:4">
+    <row r="214" spans="1:5">
       <c r="A214" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B214" s="1">
         <v>9663</v>
@@ -3513,10 +4155,13 @@
         <v>20302</v>
       </c>
       <c r="D214" s="1">
+        <v>20090</v>
+      </c>
+      <c r="E214" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="215" spans="1:4">
+    <row r="215" spans="1:5">
       <c r="A215" t="s">
         <v>9</v>
       </c>
@@ -3527,10 +4172,13 @@
         <v>19599</v>
       </c>
       <c r="D215" s="1">
+        <v>14319</v>
+      </c>
+      <c r="E215" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="216" spans="1:4">
+    <row r="216" spans="1:5">
       <c r="A216" t="s">
         <v>10</v>
       </c>
@@ -3541,10 +4189,13 @@
         <v>9492</v>
       </c>
       <c r="D216" s="1">
+        <v>10972</v>
+      </c>
+      <c r="E216" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="217" spans="1:4">
+    <row r="217" spans="1:5">
       <c r="A217" t="s">
         <v>6</v>
       </c>
@@ -3555,10 +4206,13 @@
         <v>9569</v>
       </c>
       <c r="D217" s="1">
+        <v>8233</v>
+      </c>
+      <c r="E217" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="218" spans="1:4">
+    <row r="218" spans="1:5">
       <c r="A218" t="s">
         <v>11</v>
       </c>
@@ -3569,12 +4223,15 @@
         <v>3679</v>
       </c>
       <c r="D218" s="1">
+        <v>3260</v>
+      </c>
+      <c r="E218" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="219" spans="1:4">
+    <row r="219" spans="1:5">
       <c r="A219" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B219" s="1">
         <v>2237</v>
@@ -3583,12 +4240,15 @@
         <v>4779</v>
       </c>
       <c r="D219" s="1">
+        <v>4756</v>
+      </c>
+      <c r="E219" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="220" spans="1:4">
+    <row r="220" spans="1:5">
       <c r="A220" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B220">
         <v>231</v>
@@ -3597,10 +4257,13 @@
         <v>3769</v>
       </c>
       <c r="D220" s="1">
+        <v>4531</v>
+      </c>
+      <c r="E220" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="221" spans="1:4">
+    <row r="221" spans="1:5">
       <c r="A221" t="s">
         <v>7</v>
       </c>
@@ -3611,12 +4274,15 @@
         <v>1432</v>
       </c>
       <c r="D221" s="1">
+        <v>1460</v>
+      </c>
+      <c r="E221" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="222" spans="1:4">
+    <row r="222" spans="1:5">
       <c r="A222" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B222" s="1">
         <v>238448</v>
@@ -3625,12 +4291,15 @@
         <v>209020</v>
       </c>
       <c r="D222" s="1">
+        <v>220740</v>
+      </c>
+      <c r="E222" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="223" spans="1:4">
+    <row r="223" spans="1:5">
       <c r="A223" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B223" s="1">
         <v>195407</v>
@@ -3639,10 +4308,13 @@
         <v>172748</v>
       </c>
       <c r="D223" s="1">
+        <v>182195</v>
+      </c>
+      <c r="E223" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:4">
+    <row r="224" spans="1:5">
       <c r="A224" t="s">
         <v>0</v>
       </c>
@@ -3653,12 +4325,15 @@
         <v>184811</v>
       </c>
       <c r="D224" s="1">
+        <v>193362</v>
+      </c>
+      <c r="E224" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="225" spans="1:4">
+    <row r="225" spans="1:5">
       <c r="A225" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B225" s="1">
         <v>183926</v>
@@ -3667,10 +4342,13 @@
         <v>162036</v>
       </c>
       <c r="D225" s="1">
+        <v>165903</v>
+      </c>
+      <c r="E225" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="226" spans="1:4">
+    <row r="226" spans="1:5">
       <c r="A226" t="s">
         <v>1</v>
       </c>
@@ -3681,12 +4359,15 @@
         <v>115139</v>
       </c>
       <c r="D226" s="1">
+        <v>115557</v>
+      </c>
+      <c r="E226" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="1:4">
+    <row r="227" spans="1:5">
       <c r="A227" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B227" s="1">
         <v>99253</v>
@@ -3695,10 +4376,13 @@
         <v>114342</v>
       </c>
       <c r="D227" s="1">
+        <v>129930</v>
+      </c>
+      <c r="E227" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:4">
+    <row r="228" spans="1:5">
       <c r="A228" t="s">
         <v>2</v>
       </c>
@@ -3709,10 +4393,13 @@
         <v>47140</v>
       </c>
       <c r="D228" s="1">
+        <v>46095</v>
+      </c>
+      <c r="E228" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="229" spans="1:4">
+    <row r="229" spans="1:5">
       <c r="A229" t="s">
         <v>4</v>
       </c>
@@ -3723,10 +4410,13 @@
         <v>43406</v>
       </c>
       <c r="D229" s="1">
+        <v>40672</v>
+      </c>
+      <c r="E229" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="1:4">
+    <row r="230" spans="1:5">
       <c r="A230" t="s">
         <v>3</v>
       </c>
@@ -3737,10 +4427,13 @@
         <v>49081</v>
       </c>
       <c r="D230" s="1">
+        <v>47249</v>
+      </c>
+      <c r="E230" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="231" spans="1:4">
+    <row r="231" spans="1:5">
       <c r="A231" t="s">
         <v>5</v>
       </c>
@@ -3751,12 +4444,15 @@
         <v>23854</v>
       </c>
       <c r="D231" s="1">
+        <v>25731</v>
+      </c>
+      <c r="E231" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="1:4">
+    <row r="232" spans="1:5">
       <c r="A232" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B232" s="1">
         <v>28349</v>
@@ -3765,12 +4461,15 @@
         <v>25706</v>
       </c>
       <c r="D232" s="1">
+        <v>26660</v>
+      </c>
+      <c r="E232" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="233" spans="1:4">
+    <row r="233" spans="1:5">
       <c r="A233" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B233" s="1">
         <v>26088</v>
@@ -3779,12 +4478,15 @@
         <v>24389</v>
       </c>
       <c r="D233" s="1">
+        <v>27788</v>
+      </c>
+      <c r="E233" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="234" spans="1:4">
+    <row r="234" spans="1:5">
       <c r="A234" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B234" s="1">
         <v>24567</v>
@@ -3793,12 +4495,15 @@
         <v>23558</v>
       </c>
       <c r="D234" s="1">
+        <v>23508</v>
+      </c>
+      <c r="E234" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="235" spans="1:4">
+    <row r="235" spans="1:5">
       <c r="A235" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B235" s="1">
         <v>20450</v>
@@ -3807,12 +4512,15 @@
         <v>15400</v>
       </c>
       <c r="D235" s="1">
+        <v>3950</v>
+      </c>
+      <c r="E235" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="236" spans="1:4">
+    <row r="236" spans="1:5">
       <c r="A236" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B236" s="1">
         <v>16673</v>
@@ -3821,10 +4529,13 @@
         <v>13560</v>
       </c>
       <c r="D236" s="1">
+        <v>15451</v>
+      </c>
+      <c r="E236" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="237" spans="1:4">
+    <row r="237" spans="1:5">
       <c r="A237" t="s">
         <v>9</v>
       </c>
@@ -3835,10 +4546,13 @@
         <v>13760</v>
       </c>
       <c r="D237" s="1">
+        <v>12973</v>
+      </c>
+      <c r="E237" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="238" spans="1:4">
+    <row r="238" spans="1:5">
       <c r="A238" t="s">
         <v>10</v>
       </c>
@@ -3849,10 +4563,13 @@
         <v>8151</v>
       </c>
       <c r="D238" s="1">
+        <v>6828</v>
+      </c>
+      <c r="E238" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="239" spans="1:4">
+    <row r="239" spans="1:5">
       <c r="A239" t="s">
         <v>6</v>
       </c>
@@ -3863,12 +4580,15 @@
         <v>6635</v>
       </c>
       <c r="D239" s="1">
+        <v>6283</v>
+      </c>
+      <c r="E239" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:4">
+    <row r="240" spans="1:5">
       <c r="A240" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B240" s="1">
         <v>5035</v>
@@ -3877,12 +4597,15 @@
         <v>4826</v>
       </c>
       <c r="D240" s="1">
+        <v>4382</v>
+      </c>
+      <c r="E240" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="241" spans="1:4">
+    <row r="241" spans="1:5">
       <c r="A241" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B241" s="1">
         <v>2826</v>
@@ -3891,10 +4614,13 @@
         <v>2679</v>
       </c>
       <c r="D241" s="1">
+        <v>3065</v>
+      </c>
+      <c r="E241" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="242" spans="1:4">
+    <row r="242" spans="1:5">
       <c r="A242" t="s">
         <v>11</v>
       </c>
@@ -3905,10 +4631,13 @@
         <v>3465</v>
       </c>
       <c r="D242" s="1">
+        <v>2185</v>
+      </c>
+      <c r="E242" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="243" spans="1:4">
+    <row r="243" spans="1:5">
       <c r="A243" t="s">
         <v>7</v>
       </c>
@@ -3919,12 +4648,15 @@
         <v>1330</v>
       </c>
       <c r="D243" s="1">
+        <v>1515</v>
+      </c>
+      <c r="E243" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="244" spans="1:4">
+    <row r="244" spans="1:5">
       <c r="A244" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B244" s="1">
         <v>208032</v>
@@ -3933,12 +4665,15 @@
         <v>184780</v>
       </c>
       <c r="D244" s="1">
+        <v>198386</v>
+      </c>
+      <c r="E244" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:4">
+    <row r="245" spans="1:5">
       <c r="A245" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B245" s="1">
         <v>166973</v>
@@ -3947,10 +4682,13 @@
         <v>156021</v>
       </c>
       <c r="D245" s="1">
+        <v>167056</v>
+      </c>
+      <c r="E245" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:4">
+    <row r="246" spans="1:5">
       <c r="A246" t="s">
         <v>0</v>
       </c>
@@ -3961,12 +4699,15 @@
         <v>171763</v>
       </c>
       <c r="D246" s="1">
+        <v>160411</v>
+      </c>
+      <c r="E246" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:4">
+    <row r="247" spans="1:5">
       <c r="A247" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B247" s="1">
         <v>135239</v>
@@ -3975,10 +4716,13 @@
         <v>136082</v>
       </c>
       <c r="D247" s="1">
+        <v>132803</v>
+      </c>
+      <c r="E247" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:4">
+    <row r="248" spans="1:5">
       <c r="A248" t="s">
         <v>1</v>
       </c>
@@ -3989,12 +4733,15 @@
         <v>106139</v>
       </c>
       <c r="D248" s="1">
+        <v>104542</v>
+      </c>
+      <c r="E248" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:4">
+    <row r="249" spans="1:5">
       <c r="A249" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B249" s="1">
         <v>80698</v>
@@ -4003,10 +4750,13 @@
         <v>100741</v>
       </c>
       <c r="D249" s="1">
+        <v>123538</v>
+      </c>
+      <c r="E249" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:4">
+    <row r="250" spans="1:5">
       <c r="A250" t="s">
         <v>3</v>
       </c>
@@ -4017,10 +4767,13 @@
         <v>46072</v>
       </c>
       <c r="D250" s="1">
+        <v>44357</v>
+      </c>
+      <c r="E250" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:4">
+    <row r="251" spans="1:5">
       <c r="A251" t="s">
         <v>2</v>
       </c>
@@ -4031,10 +4784,13 @@
         <v>42020</v>
       </c>
       <c r="D251" s="1">
+        <v>41242</v>
+      </c>
+      <c r="E251" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:4">
+    <row r="252" spans="1:5">
       <c r="A252" t="s">
         <v>4</v>
       </c>
@@ -4045,12 +4801,15 @@
         <v>37376</v>
       </c>
       <c r="D252" s="1">
+        <v>35628</v>
+      </c>
+      <c r="E252" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:4">
+    <row r="253" spans="1:5">
       <c r="A253" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B253" s="1">
         <v>25325</v>
@@ -4059,12 +4818,15 @@
         <v>23721</v>
       </c>
       <c r="D253" s="1">
+        <v>27498</v>
+      </c>
+      <c r="E253" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:4">
+    <row r="254" spans="1:5">
       <c r="A254" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B254" s="1">
         <v>24953</v>
@@ -4073,10 +4835,13 @@
         <v>23074</v>
       </c>
       <c r="D254" s="1">
+        <v>24744</v>
+      </c>
+      <c r="E254" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:4">
+    <row r="255" spans="1:5">
       <c r="A255" t="s">
         <v>5</v>
       </c>
@@ -4087,12 +4852,15 @@
         <v>20045</v>
       </c>
       <c r="D255" s="1">
+        <v>24962</v>
+      </c>
+      <c r="E255" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:4">
+    <row r="256" spans="1:5">
       <c r="A256" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B256" s="1">
         <v>22350</v>
@@ -4101,12 +4869,15 @@
         <v>18500</v>
       </c>
       <c r="D256" s="1">
+        <v>3750</v>
+      </c>
+      <c r="E256" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:4">
+    <row r="257" spans="1:5">
       <c r="A257" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B257" s="1">
         <v>18882</v>
@@ -4115,12 +4886,15 @@
         <v>18102</v>
       </c>
       <c r="D257" s="1">
+        <v>19016</v>
+      </c>
+      <c r="E257" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:4">
+    <row r="258" spans="1:5">
       <c r="A258" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B258" s="1">
         <v>15031</v>
@@ -4129,10 +4903,13 @@
         <v>14253</v>
       </c>
       <c r="D258" s="1">
+        <v>14511</v>
+      </c>
+      <c r="E258" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:4">
+    <row r="259" spans="1:5">
       <c r="A259" t="s">
         <v>9</v>
       </c>
@@ -4143,10 +4920,13 @@
         <v>8708</v>
       </c>
       <c r="D259" s="1">
+        <v>8480</v>
+      </c>
+      <c r="E259" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:4">
+    <row r="260" spans="1:5">
       <c r="A260" t="s">
         <v>10</v>
       </c>
@@ -4157,10 +4937,13 @@
         <v>7385</v>
       </c>
       <c r="D260" s="1">
+        <v>6446</v>
+      </c>
+      <c r="E260" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:4">
+    <row r="261" spans="1:5">
       <c r="A261" t="s">
         <v>6</v>
       </c>
@@ -4171,12 +4954,15 @@
         <v>5854</v>
       </c>
       <c r="D261" s="1">
+        <v>5567</v>
+      </c>
+      <c r="E261" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:4">
+    <row r="262" spans="1:5">
       <c r="A262" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B262" s="1">
         <v>5061</v>
@@ -4185,12 +4971,15 @@
         <v>5419</v>
       </c>
       <c r="D262" s="1">
+        <v>4816</v>
+      </c>
+      <c r="E262" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:4">
+    <row r="263" spans="1:5">
       <c r="A263" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B263" s="1">
         <v>2180</v>
@@ -4199,10 +4988,13 @@
         <v>2457</v>
       </c>
       <c r="D263" s="1">
+        <v>2937</v>
+      </c>
+      <c r="E263" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:4">
+    <row r="264" spans="1:5">
       <c r="A264" t="s">
         <v>11</v>
       </c>
@@ -4213,10 +5005,13 @@
         <v>3078</v>
       </c>
       <c r="D264" s="1">
+        <v>2604</v>
+      </c>
+      <c r="E264" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:4">
+    <row r="265" spans="1:5">
       <c r="A265" t="s">
         <v>7</v>
       </c>
@@ -4227,6 +5022,9 @@
         <v>1238</v>
       </c>
       <c r="D265" s="1">
+        <v>1486</v>
+      </c>
+      <c r="E265" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>